<commit_message>
second commit, applying Silver Meal
</commit_message>
<xml_diff>
--- a/ejemplojava.xlsx
+++ b/ejemplojava.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Planteamiento" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="137">
   <si>
     <t>Demanda</t>
   </si>
@@ -779,6 +779,33 @@
   <si>
     <t>FOQ Y L4L</t>
   </si>
+  <si>
+    <t>REQ</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ORDEN</t>
+  </si>
+  <si>
+    <t>EME indica hasta donde cubre la ultima orden</t>
+  </si>
+  <si>
+    <t>CONT indica cuando se debe colocar la siguiente orden</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ordenar</t>
+  </si>
+  <si>
+    <t>hasta</t>
+  </si>
+  <si>
+    <t>desde</t>
+  </si>
 </sst>
 </file>
 
@@ -911,7 +938,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1034,6 +1061,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1856,7 +1907,7 @@
     <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2366,6 +2417,31 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="22" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2394,6 +2470,12 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2401,6 +2483,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="20" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2583,11 +2668,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="179910192"/>
-        <c:axId val="179911760"/>
+        <c:axId val="309288728"/>
+        <c:axId val="309292256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179910192"/>
+        <c:axId val="309288728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2629,7 +2714,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179911760"/>
+        <c:crossAx val="309292256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2637,7 +2722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179911760"/>
+        <c:axId val="309292256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2688,7 +2773,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179910192"/>
+        <c:crossAx val="309288728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3806,6 +3891,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>334166</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Recorte de pantalla"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9382125" y="9153525"/>
+          <a:ext cx="5668166" cy="581106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -4186,18 +4320,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C1" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
+      <c r="C1" s="229" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
+      <c r="K1" s="229"/>
+      <c r="L1" s="229"/>
       <c r="O1">
         <f>2500*3</f>
         <v>7500</v>
@@ -4324,11 +4458,11 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E6" s="224" t="s">
+      <c r="E6" s="233" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
+      <c r="F6" s="233"/>
+      <c r="G6" s="233"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
@@ -4440,20 +4574,20 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="221" t="s">
+      <c r="C16" s="230" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="221"/>
-      <c r="E16" s="222" t="s">
+      <c r="D16" s="230"/>
+      <c r="E16" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="222"/>
-      <c r="G16" s="222"/>
+      <c r="F16" s="231"/>
+      <c r="G16" s="231"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="221" t="s">
+      <c r="M16" s="230" t="s">
         <v>16</v>
       </c>
-      <c r="N16" s="221"/>
+      <c r="N16" s="230"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
@@ -5206,7 +5340,7 @@
       <c r="K29" s="1">
         <v>8</v>
       </c>
-      <c r="M29" s="223" t="s">
+      <c r="M29" s="232" t="s">
         <v>35</v>
       </c>
       <c r="N29" s="49" t="s">
@@ -5250,7 +5384,7 @@
       <c r="K30" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="223"/>
+      <c r="M30" s="232"/>
       <c r="N30" s="10" t="s">
         <v>25</v>
       </c>
@@ -5296,7 +5430,7 @@
       <c r="K31" s="58">
         <v>0</v>
       </c>
-      <c r="M31" s="223"/>
+      <c r="M31" s="232"/>
       <c r="N31" s="10" t="s">
         <v>26</v>
       </c>
@@ -5342,7 +5476,7 @@
       <c r="K32" s="64">
         <v>0</v>
       </c>
-      <c r="M32" s="223"/>
+      <c r="M32" s="232"/>
       <c r="N32" s="10" t="s">
         <v>27</v>
       </c>
@@ -5389,7 +5523,7 @@
       <c r="K33" s="64">
         <v>0</v>
       </c>
-      <c r="M33" s="223"/>
+      <c r="M33" s="232"/>
       <c r="N33" s="10" t="s">
         <v>33</v>
       </c>
@@ -5453,7 +5587,7 @@
       <c r="K34" s="62">
         <v>0</v>
       </c>
-      <c r="M34" s="219" t="s">
+      <c r="M34" s="228" t="s">
         <v>38</v>
       </c>
       <c r="N34" s="49" t="s">
@@ -5511,7 +5645,7 @@
       <c r="K35" s="64">
         <v>0</v>
       </c>
-      <c r="M35" s="219"/>
+      <c r="M35" s="228"/>
       <c r="N35" s="10" t="s">
         <v>25</v>
       </c>
@@ -5568,7 +5702,7 @@
       <c r="K36" s="64">
         <v>0</v>
       </c>
-      <c r="M36" s="219"/>
+      <c r="M36" s="228"/>
       <c r="N36" s="10" t="s">
         <v>32</v>
       </c>
@@ -5592,7 +5726,7 @@
       <c r="AD36"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="M37" s="219"/>
+      <c r="M37" s="228"/>
       <c r="N37" s="10" t="s">
         <v>27</v>
       </c>
@@ -5620,7 +5754,7 @@
       <c r="B38" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="M38" s="219">
+      <c r="M38" s="228">
         <v>2</v>
       </c>
       <c r="N38" s="49" t="s">
@@ -5675,7 +5809,7 @@
       <c r="K39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M39" s="219"/>
+      <c r="M39" s="228"/>
       <c r="N39" s="10" t="s">
         <v>28</v>
       </c>
@@ -5728,7 +5862,7 @@
       <c r="K40" s="56">
         <v>0</v>
       </c>
-      <c r="M40" s="219" t="s">
+      <c r="M40" s="228" t="s">
         <v>41</v>
       </c>
       <c r="N40" s="49" t="s">
@@ -5775,7 +5909,7 @@
       <c r="K41" s="56">
         <v>0</v>
       </c>
-      <c r="M41" s="219"/>
+      <c r="M41" s="228"/>
       <c r="N41" s="10" t="s">
         <v>29</v>
       </c>
@@ -5821,7 +5955,7 @@
       <c r="K42" s="56">
         <v>0</v>
       </c>
-      <c r="M42" s="219"/>
+      <c r="M42" s="228"/>
       <c r="N42" s="10" t="s">
         <v>26</v>
       </c>
@@ -5867,7 +6001,7 @@
       <c r="K43" s="56">
         <v>0</v>
       </c>
-      <c r="M43" s="219"/>
+      <c r="M43" s="228"/>
       <c r="N43" s="10" t="s">
         <v>30</v>
       </c>
@@ -5913,7 +6047,7 @@
       <c r="K44" s="56">
         <v>0</v>
       </c>
-      <c r="M44" s="219"/>
+      <c r="M44" s="228"/>
       <c r="N44" s="10" t="s">
         <v>33</v>
       </c>
@@ -5963,7 +6097,7 @@
       <c r="K45" s="56">
         <v>1</v>
       </c>
-      <c r="M45" s="219"/>
+      <c r="M45" s="228"/>
       <c r="N45" s="12" t="s">
         <v>31</v>
       </c>
@@ -5976,7 +6110,7 @@
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="M46" s="219" t="s">
+      <c r="M46" s="228" t="s">
         <v>42</v>
       </c>
       <c r="N46" s="70" t="s">
@@ -5993,7 +6127,7 @@
       <c r="B47" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="M47" s="219"/>
+      <c r="M47" s="228"/>
       <c r="N47" s="10" t="s">
         <v>29</v>
       </c>
@@ -6039,7 +6173,7 @@
       <c r="K48" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="M48" s="219"/>
+      <c r="M48" s="228"/>
       <c r="N48" s="10" t="s">
         <v>32</v>
       </c>
@@ -6070,7 +6204,7 @@
       <c r="I49" s="57"/>
       <c r="J49" s="57"/>
       <c r="K49" s="57"/>
-      <c r="M49" s="219"/>
+      <c r="M49" s="228"/>
       <c r="N49" s="10" t="s">
         <v>30</v>
       </c>
@@ -6107,7 +6241,7 @@
       <c r="I50" s="61"/>
       <c r="J50" s="61"/>
       <c r="K50" s="61"/>
-      <c r="M50" s="219"/>
+      <c r="M50" s="228"/>
       <c r="N50" s="12" t="s">
         <v>31</v>
       </c>
@@ -10557,7 +10691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -10582,26 +10716,26 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="225" t="s">
+      <c r="E2" s="234" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225" t="s">
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="234" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="225"/>
-      <c r="J2" s="225"/>
-      <c r="K2" s="225" t="s">
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="K2" s="234" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="225"/>
-      <c r="M2" s="225"/>
-      <c r="N2" s="225" t="s">
+      <c r="L2" s="234"/>
+      <c r="M2" s="234"/>
+      <c r="N2" s="234" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="225"/>
-      <c r="P2" s="225"/>
+      <c r="O2" s="234"/>
+      <c r="P2" s="234"/>
       <c r="R2" s="113"/>
       <c r="S2" s="114"/>
       <c r="T2" s="115"/>
@@ -11287,26 +11421,26 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="225" t="s">
+      <c r="E18" s="234" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="225"/>
-      <c r="G18" s="225"/>
-      <c r="H18" s="225" t="s">
+      <c r="F18" s="234"/>
+      <c r="G18" s="234"/>
+      <c r="H18" s="234" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="225"/>
-      <c r="J18" s="225"/>
-      <c r="K18" s="225" t="s">
+      <c r="I18" s="234"/>
+      <c r="J18" s="234"/>
+      <c r="K18" s="234" t="s">
         <v>74</v>
       </c>
-      <c r="L18" s="225"/>
-      <c r="M18" s="225"/>
-      <c r="N18" s="225" t="s">
+      <c r="L18" s="234"/>
+      <c r="M18" s="234"/>
+      <c r="N18" s="234" t="s">
         <v>75</v>
       </c>
-      <c r="O18" s="225"/>
-      <c r="P18" s="225"/>
+      <c r="O18" s="234"/>
+      <c r="P18" s="234"/>
       <c r="R18" s="145"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -12962,11 +13096,11 @@
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
       <c r="I38" s="16"/>
-      <c r="K38" s="226">
+      <c r="K38" s="235">
         <f>H37+H18+'Nivel 1'!N14</f>
         <v>88250</v>
       </c>
-      <c r="L38" s="226"/>
+      <c r="L38" s="235"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -13051,14 +13185,14 @@
       <c r="I2">
         <v>50</v>
       </c>
-      <c r="S2" s="227" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="227"/>
-      <c r="U2" s="227" t="s">
+      <c r="S2" s="236" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="236"/>
+      <c r="U2" s="236" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="227"/>
+      <c r="V2" s="236"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E3">
@@ -13112,39 +13246,39 @@
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(0,1000)</f>
-        <v>498</v>
+        <v>985</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:M10" ca="1" si="0">RANDBETWEEN(0,1000)</f>
-        <v>935</v>
+        <v>188</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>478</v>
+        <v>633</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <v>443</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>481</v>
+        <v>390</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>799</v>
+        <v>356</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>410</v>
+        <v>720</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>604</v>
+        <v>18</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>282</v>
+        <v>863</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -13154,39 +13288,39 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E10" ca="1" si="1">RANDBETWEEN(0,1000)</f>
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>488</v>
+        <v>661</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>432</v>
+        <v>103</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>258</v>
+        <v>356</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>442</v>
+        <v>895</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>773</v>
+        <v>263</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>732</v>
+        <v>294</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>912</v>
+        <v>440</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -13196,39 +13330,39 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>262</v>
+        <v>878</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>789</v>
+        <v>88</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>541</v>
+        <v>855</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>696</v>
+        <v>549</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>768</v>
+        <v>99</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>344</v>
+        <v>32</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>415</v>
+        <v>721</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>995</v>
+        <v>313</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>868</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -13238,39 +13372,39 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>710</v>
+        <v>200</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>221</v>
+        <v>659</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>685</v>
+        <v>816</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>779</v>
+        <v>606</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>776</v>
+        <v>296</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>795</v>
+        <v>642</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>464</v>
+        <v>60</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>763</v>
+        <v>841</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
-        <v>771</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -13280,11 +13414,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>219</v>
+        <v>939</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>904</v>
+        <v>283</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
@@ -13292,27 +13426,27 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>611</v>
+        <v>327</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>664</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>521</v>
+        <v>227</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>862</v>
+        <v>615</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>459</v>
+        <v>585</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
-        <v>575</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -13322,39 +13456,39 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>399</v>
+        <v>305</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>630</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>725</v>
+        <v>911</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>101</v>
+        <v>773</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>494</v>
+        <v>229</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>362</v>
+        <v>847</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>380</v>
+        <v>250</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="0"/>
-        <v>723</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -13367,39 +13501,39 @@
       </c>
       <c r="E13">
         <f t="shared" ref="E13:M13" ca="1" si="3">E5*$A13</f>
-        <v>498</v>
+        <v>985</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="3"/>
-        <v>935</v>
+        <v>188</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="3"/>
-        <v>478</v>
+        <v>633</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="3"/>
-        <v>158</v>
+        <v>443</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>481</v>
+        <v>390</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>799</v>
+        <v>356</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="3"/>
-        <v>410</v>
+        <v>720</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>604</v>
+        <v>18</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="3"/>
-        <v>282</v>
+        <v>863</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -13412,39 +13546,39 @@
       </c>
       <c r="E14">
         <f t="shared" ref="E14:M14" ca="1" si="4">E6*$A14</f>
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="4"/>
-        <v>244</v>
+        <v>330.5</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="4"/>
-        <v>216</v>
+        <v>51.5</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="4"/>
-        <v>129</v>
+        <v>178</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="4"/>
-        <v>221</v>
+        <v>447.5</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>386.5</v>
+        <v>131.5</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>366</v>
+        <v>147</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="4"/>
-        <v>456</v>
+        <v>220</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="4"/>
-        <v>40.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -13457,39 +13591,39 @@
       </c>
       <c r="E15">
         <f t="shared" ref="E15:M15" ca="1" si="5">E7*$A15</f>
-        <v>262</v>
+        <v>878</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="5"/>
-        <v>789</v>
+        <v>88</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="5"/>
-        <v>541</v>
+        <v>855</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="5"/>
-        <v>696</v>
+        <v>549</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="5"/>
-        <v>768</v>
+        <v>99</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="5"/>
-        <v>344</v>
+        <v>32</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="5"/>
-        <v>415</v>
+        <v>721</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="5"/>
-        <v>995</v>
+        <v>313</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
-        <v>868</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -13502,39 +13636,39 @@
       </c>
       <c r="E16">
         <f t="shared" ref="E16:M16" ca="1" si="6">E8*$A16</f>
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="6"/>
-        <v>22.1</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="6"/>
-        <v>68.5</v>
+        <v>81.600000000000009</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="6"/>
-        <v>77.900000000000006</v>
+        <v>60.6</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="6"/>
-        <v>77.600000000000009</v>
+        <v>29.6</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="6"/>
-        <v>79.5</v>
+        <v>64.2</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="6"/>
-        <v>46.400000000000006</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="6"/>
-        <v>76.3</v>
+        <v>84.100000000000009</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="6"/>
-        <v>77.100000000000009</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -13547,11 +13681,11 @@
       </c>
       <c r="E17">
         <f t="shared" ref="E17:M17" ca="1" si="7">E9*$A17</f>
-        <v>438</v>
+        <v>1878</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="7"/>
-        <v>1808</v>
+        <v>566</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="7"/>
@@ -13559,27 +13693,27 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="7"/>
-        <v>1222</v>
+        <v>654</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="7"/>
-        <v>110</v>
+        <v>1328</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="7"/>
-        <v>1042</v>
+        <v>454</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="7"/>
-        <v>1724</v>
+        <v>1230</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="7"/>
-        <v>918</v>
+        <v>1170</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="7"/>
-        <v>1150</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -13592,39 +13726,39 @@
       </c>
       <c r="E18">
         <f t="shared" ref="E18:M18" ca="1" si="8">E10*$A18</f>
-        <v>399</v>
+        <v>305</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="8"/>
-        <v>11</v>
+        <v>630</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="8"/>
-        <v>725</v>
+        <v>911</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="8"/>
-        <v>101</v>
+        <v>773</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="8"/>
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="8"/>
-        <v>494</v>
+        <v>229</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="8"/>
-        <v>362</v>
+        <v>847</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="8"/>
-        <v>380</v>
+        <v>250</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="8"/>
-        <v>723</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -13634,39 +13768,39 @@
       </c>
       <c r="E19" s="16">
         <f ca="1">SUM(E13:E18)</f>
-        <v>1722</v>
+        <v>4092</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" ref="F19:M19" ca="1" si="9">SUM(F13:F18)</f>
-        <v>3809.1</v>
+        <v>1868.4</v>
       </c>
       <c r="G19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>3948.5</v>
+        <v>4452.1000000000004</v>
       </c>
       <c r="H19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>2383.9</v>
+        <v>2657.6</v>
       </c>
       <c r="I19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>2425.6</v>
+        <v>3035.1</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>3145</v>
+        <v>1266.7</v>
       </c>
       <c r="K19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>3323.4</v>
+        <v>3671</v>
       </c>
       <c r="L19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>3429.3</v>
+        <v>2055.1</v>
       </c>
       <c r="M19" s="16">
         <f t="shared" ca="1" si="9"/>
-        <v>3140.6</v>
+        <v>3439.6</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -13901,14 +14035,14 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D56" s="227" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" s="227"/>
-      <c r="F56" s="227" t="s">
+      <c r="D56" s="236" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="236"/>
+      <c r="F56" s="236" t="s">
         <v>3</v>
       </c>
-      <c r="G56" s="227"/>
+      <c r="G56" s="236"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="186" t="s">
@@ -14634,20 +14768,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="228" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
+      <c r="A2" s="237" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -14916,20 +15050,20 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="228" t="s">
+      <c r="A10" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="228"/>
-      <c r="C10" s="228"/>
-      <c r="D10" s="228"/>
-      <c r="E10" s="228"/>
-      <c r="F10" s="228"/>
-      <c r="G10" s="228"/>
-      <c r="H10" s="228"/>
-      <c r="I10" s="228"/>
-      <c r="J10" s="228"/>
-      <c r="K10" s="228"/>
-      <c r="L10" s="228"/>
+      <c r="B10" s="237"/>
+      <c r="C10" s="237"/>
+      <c r="D10" s="237"/>
+      <c r="E10" s="237"/>
+      <c r="F10" s="237"/>
+      <c r="G10" s="237"/>
+      <c r="H10" s="237"/>
+      <c r="I10" s="237"/>
+      <c r="J10" s="237"/>
+      <c r="K10" s="237"/>
+      <c r="L10" s="237"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -15163,13 +15297,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y120"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="S84" sqref="S84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -15319,28 +15464,28 @@
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
-      <c r="C7" s="229" t="s">
+      <c r="C7" s="240" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229" t="s">
+      <c r="D7" s="240"/>
+      <c r="E7" s="240"/>
+      <c r="F7" s="240" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="229"/>
-      <c r="H7" s="229"/>
+      <c r="G7" s="240"/>
+      <c r="H7" s="240"/>
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
-      <c r="P7" s="229" t="s">
+      <c r="P7" s="240" t="s">
         <v>111</v>
       </c>
-      <c r="Q7" s="229"/>
-      <c r="R7" s="229"/>
-      <c r="S7" s="229" t="s">
+      <c r="Q7" s="240"/>
+      <c r="R7" s="240"/>
+      <c r="S7" s="240" t="s">
         <v>106</v>
       </c>
-      <c r="T7" s="229"/>
-      <c r="U7" s="229"/>
+      <c r="T7" s="240"/>
+      <c r="U7" s="240"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -16061,14 +16206,14 @@
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="230" t="s">
+      <c r="F27" s="241" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="231"/>
-      <c r="H27" s="230" t="s">
+      <c r="G27" s="242"/>
+      <c r="H27" s="241" t="s">
         <v>106</v>
       </c>
-      <c r="I27" s="231"/>
+      <c r="I27" s="242"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
@@ -16213,7 +16358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D33" s="186">
         <v>4</v>
       </c>
@@ -16242,7 +16387,7 @@
         <v>8910</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D34" s="186">
         <v>5</v>
       </c>
@@ -16264,7 +16409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D35" s="186">
         <v>6</v>
       </c>
@@ -16286,7 +16431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D36" s="186">
         <v>7</v>
       </c>
@@ -16307,7 +16452,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D37" s="186">
         <v>8</v>
       </c>
@@ -16325,7 +16470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D38" s="186">
         <v>9</v>
       </c>
@@ -16341,12 +16486,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -16381,7 +16526,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -16416,7 +16561,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>945</v>
       </c>
@@ -16451,7 +16596,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ref="A46:B46" si="10">A43-A44</f>
         <v>-945</v>
@@ -16496,8 +16641,2033 @@
         <v>114</v>
       </c>
     </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="220"/>
+      <c r="B48" s="220"/>
+      <c r="C48" s="220"/>
+      <c r="D48" s="220"/>
+      <c r="E48" s="220"/>
+      <c r="F48" s="220"/>
+      <c r="G48" s="220"/>
+      <c r="H48" s="220"/>
+      <c r="I48" s="220"/>
+      <c r="J48" s="220"/>
+      <c r="K48" s="220"/>
+      <c r="L48" s="220"/>
+      <c r="M48" s="220"/>
+      <c r="N48" s="220"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49" s="221" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="223" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="223" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="219">
+        <v>56</v>
+      </c>
+      <c r="E49" s="223" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="219">
+        <v>1500</v>
+      </c>
+      <c r="G49" s="220"/>
+      <c r="H49" s="220"/>
+      <c r="I49" s="220"/>
+      <c r="J49" s="220"/>
+      <c r="K49" s="220"/>
+      <c r="L49" s="220"/>
+      <c r="M49" s="220"/>
+      <c r="N49" s="220"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" s="221">
+        <v>0</v>
+      </c>
+      <c r="B50" s="221">
+        <v>0</v>
+      </c>
+      <c r="C50" s="221">
+        <v>0</v>
+      </c>
+      <c r="D50" s="221">
+        <v>1770</v>
+      </c>
+      <c r="E50" s="221">
+        <v>1800</v>
+      </c>
+      <c r="F50" s="221">
+        <v>0</v>
+      </c>
+      <c r="G50" s="221">
+        <v>1200</v>
+      </c>
+      <c r="H50" s="221">
+        <v>0</v>
+      </c>
+      <c r="I50" s="221">
+        <v>600</v>
+      </c>
+      <c r="J50" s="221">
+        <v>0</v>
+      </c>
+      <c r="K50" s="239" t="s">
+        <v>128</v>
+      </c>
+      <c r="L50" s="221"/>
+      <c r="M50" s="225" t="s">
+        <v>135</v>
+      </c>
+      <c r="N50" s="221">
+        <f>B62-1+0</f>
+        <v>3</v>
+      </c>
+      <c r="W50" s="238"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="221">
+        <v>1</v>
+      </c>
+      <c r="B51" s="221">
+        <v>2</v>
+      </c>
+      <c r="C51" s="221">
+        <v>3</v>
+      </c>
+      <c r="D51" s="221">
+        <v>4</v>
+      </c>
+      <c r="E51" s="221">
+        <v>5</v>
+      </c>
+      <c r="F51" s="221">
+        <v>6</v>
+      </c>
+      <c r="G51" s="221">
+        <v>7</v>
+      </c>
+      <c r="H51" s="221">
+        <v>8</v>
+      </c>
+      <c r="I51" s="221">
+        <v>9</v>
+      </c>
+      <c r="J51" s="221">
+        <v>10</v>
+      </c>
+      <c r="K51" s="239"/>
+      <c r="L51" s="221"/>
+      <c r="M51" s="226" t="s">
+        <v>136</v>
+      </c>
+      <c r="N51" s="221">
+        <f>N50+1</f>
+        <v>4</v>
+      </c>
+      <c r="W51" s="238"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52" s="221"/>
+      <c r="B52" s="221"/>
+      <c r="C52" s="221"/>
+      <c r="D52" s="221"/>
+      <c r="E52" s="221"/>
+      <c r="F52" s="221"/>
+      <c r="G52" s="221"/>
+      <c r="H52" s="221"/>
+      <c r="I52" s="221"/>
+      <c r="J52" s="221"/>
+      <c r="K52" s="221">
+        <f>SUM(A50:J50)</f>
+        <v>5370</v>
+      </c>
+      <c r="L52" s="221"/>
+      <c r="M52" s="221" t="s">
+        <v>133</v>
+      </c>
+      <c r="N52" s="221"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53" s="221" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="221"/>
+      <c r="C53" s="221"/>
+      <c r="D53" s="221"/>
+      <c r="E53" s="221"/>
+      <c r="F53" s="221"/>
+      <c r="G53" s="221"/>
+      <c r="H53" s="221"/>
+      <c r="I53" s="221"/>
+      <c r="J53" s="221"/>
+      <c r="K53" s="221"/>
+      <c r="L53" s="221"/>
+      <c r="M53" s="221"/>
+      <c r="N53" s="221"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54" s="221">
+        <f>A50+B50+C50</f>
+        <v>0</v>
+      </c>
+      <c r="B54" s="221">
+        <v>0</v>
+      </c>
+      <c r="C54" s="221">
+        <v>0</v>
+      </c>
+      <c r="D54" s="221">
+        <f>D50</f>
+        <v>1770</v>
+      </c>
+      <c r="E54" s="221">
+        <f>E50+F50</f>
+        <v>1800</v>
+      </c>
+      <c r="F54" s="221">
+        <f>F50</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="221">
+        <f>G50+H50</f>
+        <v>1200</v>
+      </c>
+      <c r="H54" s="221">
+        <v>0</v>
+      </c>
+      <c r="I54" s="221">
+        <f>I50+J50</f>
+        <v>600</v>
+      </c>
+      <c r="J54" s="221">
+        <v>0</v>
+      </c>
+      <c r="K54" s="221">
+        <f>SUM(A54:J54)</f>
+        <v>5370</v>
+      </c>
+      <c r="L54" s="221"/>
+      <c r="M54" s="221"/>
+      <c r="N54" s="221"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55" s="221">
+        <v>1</v>
+      </c>
+      <c r="B55" s="221">
+        <v>2</v>
+      </c>
+      <c r="C55" s="221">
+        <v>3</v>
+      </c>
+      <c r="D55" s="221">
+        <v>4</v>
+      </c>
+      <c r="E55" s="221">
+        <v>5</v>
+      </c>
+      <c r="F55" s="221">
+        <v>6</v>
+      </c>
+      <c r="G55" s="221">
+        <v>7</v>
+      </c>
+      <c r="H55" s="221">
+        <v>8</v>
+      </c>
+      <c r="I55" s="221">
+        <v>9</v>
+      </c>
+      <c r="J55" s="221">
+        <v>10</v>
+      </c>
+      <c r="K55" s="220"/>
+      <c r="L55" s="220"/>
+      <c r="M55" s="220"/>
+      <c r="N55" s="220"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56" s="220"/>
+      <c r="B56" s="220"/>
+      <c r="C56" s="220"/>
+      <c r="D56" s="220"/>
+      <c r="E56" s="220"/>
+      <c r="F56" s="220"/>
+      <c r="G56" s="220"/>
+      <c r="H56" s="220"/>
+      <c r="I56" s="220"/>
+      <c r="J56" s="220"/>
+      <c r="K56" s="220"/>
+      <c r="L56" s="220"/>
+      <c r="M56" s="220"/>
+      <c r="N56" s="220"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A57" s="221" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="220"/>
+      <c r="C57" s="220"/>
+      <c r="D57" s="220"/>
+      <c r="E57" s="220"/>
+      <c r="F57" s="220"/>
+      <c r="G57" s="220"/>
+      <c r="H57" s="220"/>
+      <c r="I57" s="220"/>
+      <c r="J57" s="220"/>
+      <c r="K57" s="221"/>
+      <c r="L57" s="221"/>
+      <c r="M57" s="221"/>
+      <c r="N57" s="221"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A58" s="227">
+        <v>0</v>
+      </c>
+      <c r="B58" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="221">
+        <v>1</v>
+      </c>
+      <c r="D58" s="221">
+        <v>2</v>
+      </c>
+      <c r="E58" s="221">
+        <v>3</v>
+      </c>
+      <c r="F58" s="221">
+        <v>4</v>
+      </c>
+      <c r="G58" s="221">
+        <v>5</v>
+      </c>
+      <c r="H58" s="221">
+        <v>6</v>
+      </c>
+      <c r="I58" s="221">
+        <v>7</v>
+      </c>
+      <c r="J58" s="221">
+        <v>8</v>
+      </c>
+      <c r="K58" s="221">
+        <v>9</v>
+      </c>
+      <c r="L58" s="221">
+        <v>10</v>
+      </c>
+      <c r="M58" s="221"/>
+      <c r="N58" s="221"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A59" s="226">
+        <v>1</v>
+      </c>
+      <c r="B59" s="221">
+        <v>1</v>
+      </c>
+      <c r="C59" s="222">
+        <v>0</v>
+      </c>
+      <c r="D59" s="222"/>
+      <c r="E59" s="222"/>
+      <c r="F59" s="222"/>
+      <c r="G59" s="222"/>
+      <c r="H59" s="222"/>
+      <c r="I59" s="222"/>
+      <c r="J59" s="222"/>
+      <c r="K59" s="222"/>
+      <c r="L59" s="222"/>
+      <c r="M59" s="243">
+        <f t="shared" ref="M59:M60" si="12">($F$49+SUM(C59:L59))/B59</f>
+        <v>1500</v>
+      </c>
+      <c r="N59" s="221"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60" s="221">
+        <v>2</v>
+      </c>
+      <c r="B60" s="221">
+        <v>2</v>
+      </c>
+      <c r="C60" s="222">
+        <f>0*B50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="222">
+        <f>C$58*B50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E60" s="222"/>
+      <c r="F60" s="222"/>
+      <c r="G60" s="222"/>
+      <c r="H60" s="222"/>
+      <c r="I60" s="222"/>
+      <c r="J60" s="222"/>
+      <c r="K60" s="222"/>
+      <c r="L60" s="222"/>
+      <c r="M60" s="243">
+        <f t="shared" si="12"/>
+        <v>750</v>
+      </c>
+      <c r="N60" s="221" t="str">
+        <f t="shared" ref="N60:N61" si="13">IF(M60&gt;M59,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A61" s="227">
+        <v>3</v>
+      </c>
+      <c r="B61" s="221">
+        <v>3</v>
+      </c>
+      <c r="C61" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D61" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="222">
+        <f>D$58*C$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="222"/>
+      <c r="G61" s="222"/>
+      <c r="H61" s="222"/>
+      <c r="I61" s="222"/>
+      <c r="J61" s="222"/>
+      <c r="K61" s="222"/>
+      <c r="L61" s="222"/>
+      <c r="M61" s="243">
+        <f>($F$49+SUM(C61:L61))/B61</f>
+        <v>500</v>
+      </c>
+      <c r="N61" s="221" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62" s="226">
+        <v>4</v>
+      </c>
+      <c r="B62" s="221">
+        <v>4</v>
+      </c>
+      <c r="C62" s="222">
+        <f>0*A$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D62" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="222">
+        <f>D$58*C$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="222">
+        <f>E$58*D$50*$D$49</f>
+        <v>297360</v>
+      </c>
+      <c r="G62" s="222"/>
+      <c r="H62" s="222"/>
+      <c r="I62" s="222"/>
+      <c r="J62" s="222"/>
+      <c r="K62" s="222"/>
+      <c r="L62" s="222"/>
+      <c r="M62" s="243">
+        <f>($F$49+SUM(C62:L62))/B62</f>
+        <v>74715</v>
+      </c>
+      <c r="N62" s="221" t="str">
+        <f>IF(M62&gt;M61,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A63" s="221"/>
+      <c r="B63" s="221"/>
+      <c r="C63" s="222"/>
+      <c r="D63" s="222"/>
+      <c r="E63" s="222"/>
+      <c r="F63" s="222"/>
+      <c r="G63" s="222"/>
+      <c r="H63" s="222"/>
+      <c r="I63" s="222"/>
+      <c r="J63" s="222"/>
+      <c r="K63" s="222"/>
+      <c r="L63" s="222"/>
+      <c r="M63" s="222"/>
+      <c r="N63" s="221"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A64" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="221">
+        <v>1</v>
+      </c>
+      <c r="D64" s="221">
+        <v>2</v>
+      </c>
+      <c r="E64" s="221">
+        <v>3</v>
+      </c>
+      <c r="F64" s="221">
+        <v>4</v>
+      </c>
+      <c r="G64" s="221">
+        <v>5</v>
+      </c>
+      <c r="H64" s="221">
+        <v>6</v>
+      </c>
+      <c r="I64" s="221">
+        <v>7</v>
+      </c>
+      <c r="J64" s="221">
+        <v>8</v>
+      </c>
+      <c r="K64" s="221">
+        <v>9</v>
+      </c>
+      <c r="L64" s="221">
+        <v>10</v>
+      </c>
+      <c r="M64" s="221"/>
+      <c r="N64" s="221"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="227">
+        <v>4</v>
+      </c>
+      <c r="B65" s="221">
+        <v>1</v>
+      </c>
+      <c r="C65" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="222"/>
+      <c r="E65" s="222"/>
+      <c r="F65" s="222"/>
+      <c r="G65" s="222"/>
+      <c r="H65" s="222"/>
+      <c r="I65" s="222"/>
+      <c r="J65" s="222"/>
+      <c r="K65" s="222"/>
+      <c r="L65" s="222"/>
+      <c r="M65" s="243">
+        <f t="shared" ref="M65:M66" si="14">($F$49+SUM(C65:L65))/B65</f>
+        <v>1500</v>
+      </c>
+      <c r="N65" s="221"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="226">
+        <v>5</v>
+      </c>
+      <c r="B66" s="221">
+        <v>2</v>
+      </c>
+      <c r="C66" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="222">
+        <f>E$50*$D$49*C$64</f>
+        <v>100800</v>
+      </c>
+      <c r="E66" s="222"/>
+      <c r="F66" s="222"/>
+      <c r="G66" s="222"/>
+      <c r="H66" s="222"/>
+      <c r="I66" s="222"/>
+      <c r="J66" s="222"/>
+      <c r="K66" s="222"/>
+      <c r="L66" s="222"/>
+      <c r="M66" s="243">
+        <f>($F$49+SUM(C66:L66))/B66</f>
+        <v>51150</v>
+      </c>
+      <c r="N66" s="221" t="str">
+        <f t="shared" ref="N66" si="15">IF(M66&gt;M65,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="221"/>
+      <c r="B67" s="221"/>
+      <c r="C67" s="222"/>
+      <c r="D67" s="222"/>
+      <c r="E67" s="222"/>
+      <c r="F67" s="222"/>
+      <c r="G67" s="222"/>
+      <c r="H67" s="222"/>
+      <c r="I67" s="222"/>
+      <c r="J67" s="222"/>
+      <c r="K67" s="222"/>
+      <c r="L67" s="222"/>
+      <c r="M67" s="222"/>
+      <c r="N67" s="221"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="221">
+        <v>1</v>
+      </c>
+      <c r="D68" s="221">
+        <v>2</v>
+      </c>
+      <c r="E68" s="221">
+        <v>3</v>
+      </c>
+      <c r="F68" s="221">
+        <v>4</v>
+      </c>
+      <c r="G68" s="221">
+        <v>5</v>
+      </c>
+      <c r="H68" s="221">
+        <v>6</v>
+      </c>
+      <c r="I68" s="221">
+        <v>7</v>
+      </c>
+      <c r="J68" s="221">
+        <v>8</v>
+      </c>
+      <c r="K68" s="221">
+        <v>9</v>
+      </c>
+      <c r="L68" s="221">
+        <v>10</v>
+      </c>
+      <c r="M68" s="221"/>
+      <c r="N68" s="221"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="221">
+        <v>5</v>
+      </c>
+      <c r="B69" s="221">
+        <v>1</v>
+      </c>
+      <c r="C69" s="222">
+        <v>0</v>
+      </c>
+      <c r="D69" s="222"/>
+      <c r="E69" s="222"/>
+      <c r="F69" s="222"/>
+      <c r="G69" s="222"/>
+      <c r="H69" s="222"/>
+      <c r="I69" s="222"/>
+      <c r="J69" s="222"/>
+      <c r="K69" s="222"/>
+      <c r="L69" s="222"/>
+      <c r="M69" s="243">
+        <f t="shared" ref="M69:M70" si="16">($F$49+SUM(C69:L69))/B69</f>
+        <v>1500</v>
+      </c>
+      <c r="N69" s="221"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="227">
+        <v>6</v>
+      </c>
+      <c r="B70" s="221">
+        <v>2</v>
+      </c>
+      <c r="C70" s="222">
+        <v>0</v>
+      </c>
+      <c r="D70" s="222">
+        <f>F$50*$D$49*C$68</f>
+        <v>0</v>
+      </c>
+      <c r="E70" s="222"/>
+      <c r="F70" s="222"/>
+      <c r="G70" s="222"/>
+      <c r="H70" s="222"/>
+      <c r="I70" s="222"/>
+      <c r="J70" s="222"/>
+      <c r="K70" s="222"/>
+      <c r="L70" s="222"/>
+      <c r="M70" s="243">
+        <f t="shared" si="16"/>
+        <v>750</v>
+      </c>
+      <c r="N70" s="221" t="str">
+        <f>IF(M70&gt;M69,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="226">
+        <v>7</v>
+      </c>
+      <c r="B71" s="221">
+        <v>3</v>
+      </c>
+      <c r="C71" s="222">
+        <v>0</v>
+      </c>
+      <c r="D71" s="222">
+        <f>F$50*$D$49*C$68</f>
+        <v>0</v>
+      </c>
+      <c r="E71" s="222">
+        <f>G$50*$D$49*D$68</f>
+        <v>134400</v>
+      </c>
+      <c r="F71" s="222"/>
+      <c r="G71" s="222"/>
+      <c r="H71" s="222"/>
+      <c r="I71" s="222"/>
+      <c r="J71" s="222"/>
+      <c r="K71" s="222"/>
+      <c r="L71" s="222"/>
+      <c r="M71" s="243">
+        <f t="shared" ref="M71" si="17">($F$49+SUM(C71:L71))/B71</f>
+        <v>45300</v>
+      </c>
+      <c r="N71" s="221" t="str">
+        <f>IF(M71&gt;M70,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="221"/>
+      <c r="B72" s="221"/>
+      <c r="C72" s="222"/>
+      <c r="D72" s="222"/>
+      <c r="E72" s="222"/>
+      <c r="F72" s="222"/>
+      <c r="G72" s="222"/>
+      <c r="H72" s="222"/>
+      <c r="I72" s="222"/>
+      <c r="J72" s="222"/>
+      <c r="K72" s="222"/>
+      <c r="L72" s="222"/>
+      <c r="M72" s="222"/>
+      <c r="N72" s="221"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="221">
+        <v>1</v>
+      </c>
+      <c r="D73" s="221">
+        <v>2</v>
+      </c>
+      <c r="E73" s="221">
+        <v>3</v>
+      </c>
+      <c r="F73" s="221">
+        <v>4</v>
+      </c>
+      <c r="G73" s="221">
+        <v>5</v>
+      </c>
+      <c r="H73" s="221">
+        <v>6</v>
+      </c>
+      <c r="I73" s="221">
+        <v>7</v>
+      </c>
+      <c r="J73" s="221">
+        <v>8</v>
+      </c>
+      <c r="K73" s="221">
+        <v>9</v>
+      </c>
+      <c r="L73" s="221">
+        <v>10</v>
+      </c>
+      <c r="M73" s="221"/>
+      <c r="N73" s="221"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="221">
+        <v>7</v>
+      </c>
+      <c r="B74" s="221">
+        <v>1</v>
+      </c>
+      <c r="C74" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D74" s="222"/>
+      <c r="E74" s="222"/>
+      <c r="F74" s="222"/>
+      <c r="G74" s="222"/>
+      <c r="H74" s="222"/>
+      <c r="I74" s="222"/>
+      <c r="J74" s="222"/>
+      <c r="K74" s="222"/>
+      <c r="L74" s="222"/>
+      <c r="M74" s="243">
+        <f t="shared" ref="M74:M75" si="18">($F$49+SUM(C74:L74))/B74</f>
+        <v>1500</v>
+      </c>
+      <c r="N74" s="221"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="227">
+        <v>8</v>
+      </c>
+      <c r="B75" s="221">
+        <v>2</v>
+      </c>
+      <c r="C75" s="222">
+        <v>0</v>
+      </c>
+      <c r="D75" s="222">
+        <f>H$50*$D$49*C$73</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="222"/>
+      <c r="F75" s="222"/>
+      <c r="G75" s="222"/>
+      <c r="H75" s="222"/>
+      <c r="I75" s="222"/>
+      <c r="J75" s="222"/>
+      <c r="K75" s="222"/>
+      <c r="L75" s="222"/>
+      <c r="M75" s="243">
+        <f t="shared" si="18"/>
+        <v>750</v>
+      </c>
+      <c r="N75" s="221" t="str">
+        <f>IF(M75&gt;M74,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="226">
+        <v>9</v>
+      </c>
+      <c r="B76" s="221">
+        <v>3</v>
+      </c>
+      <c r="C76" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D76" s="222">
+        <f>H$50*$D$49*C$73</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="222">
+        <f>I$50*$D$49*D$73</f>
+        <v>67200</v>
+      </c>
+      <c r="F76" s="222"/>
+      <c r="G76" s="222"/>
+      <c r="H76" s="222"/>
+      <c r="I76" s="222"/>
+      <c r="J76" s="222"/>
+      <c r="K76" s="222"/>
+      <c r="L76" s="222"/>
+      <c r="M76" s="243">
+        <f t="shared" ref="M76" si="19">($F$49+SUM(C76:L76))/B76</f>
+        <v>22900</v>
+      </c>
+      <c r="N76" s="221" t="str">
+        <f>IF(M76&gt;M75,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="221"/>
+      <c r="B77" s="221"/>
+      <c r="C77" s="222"/>
+      <c r="D77" s="222"/>
+      <c r="E77" s="222"/>
+      <c r="F77" s="222"/>
+      <c r="G77" s="222"/>
+      <c r="H77" s="222"/>
+      <c r="I77" s="222"/>
+      <c r="J77" s="222"/>
+      <c r="K77" s="222"/>
+      <c r="L77" s="222"/>
+      <c r="M77" s="222"/>
+      <c r="N77" s="221"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="221">
+        <v>1</v>
+      </c>
+      <c r="D78" s="221">
+        <v>2</v>
+      </c>
+      <c r="E78" s="221">
+        <v>3</v>
+      </c>
+      <c r="F78" s="221">
+        <v>4</v>
+      </c>
+      <c r="G78" s="221">
+        <v>5</v>
+      </c>
+      <c r="H78" s="221">
+        <v>6</v>
+      </c>
+      <c r="I78" s="221">
+        <v>7</v>
+      </c>
+      <c r="J78" s="221">
+        <v>8</v>
+      </c>
+      <c r="K78" s="221">
+        <v>9</v>
+      </c>
+      <c r="L78" s="221">
+        <v>10</v>
+      </c>
+      <c r="M78" s="221"/>
+      <c r="N78" s="221"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="221">
+        <v>9</v>
+      </c>
+      <c r="B79" s="221">
+        <v>1</v>
+      </c>
+      <c r="C79" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D79" s="222"/>
+      <c r="E79" s="222"/>
+      <c r="F79" s="222"/>
+      <c r="G79" s="222"/>
+      <c r="H79" s="222"/>
+      <c r="I79" s="222"/>
+      <c r="J79" s="222"/>
+      <c r="K79" s="222"/>
+      <c r="L79" s="222"/>
+      <c r="M79" s="222">
+        <f t="shared" ref="M79:M80" si="20">($F$49+SUM(C79:L79))/B79</f>
+        <v>1500</v>
+      </c>
+      <c r="N79" s="221"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="227">
+        <v>10</v>
+      </c>
+      <c r="B80" s="221">
+        <v>2</v>
+      </c>
+      <c r="C80" s="222">
+        <v>0</v>
+      </c>
+      <c r="D80" s="222">
+        <f>J$50*$D$49*C$78</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="222"/>
+      <c r="F80" s="222"/>
+      <c r="G80" s="222"/>
+      <c r="H80" s="222"/>
+      <c r="I80" s="222"/>
+      <c r="J80" s="222"/>
+      <c r="K80" s="222"/>
+      <c r="L80" s="222"/>
+      <c r="M80" s="222">
+        <f t="shared" si="20"/>
+        <v>750</v>
+      </c>
+      <c r="N80" s="221" t="str">
+        <f>IF(M80&gt;M79,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="221"/>
+      <c r="B81" s="221"/>
+      <c r="C81" s="222"/>
+      <c r="D81" s="222"/>
+      <c r="E81" s="222"/>
+      <c r="F81" s="222"/>
+      <c r="G81" s="222"/>
+      <c r="H81" s="222"/>
+      <c r="I81" s="222"/>
+      <c r="J81" s="222"/>
+      <c r="K81" s="222"/>
+      <c r="L81" s="222"/>
+      <c r="M81" s="222"/>
+      <c r="N81" s="221"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="220"/>
+      <c r="B82" s="220"/>
+      <c r="C82" s="220"/>
+      <c r="D82" s="220"/>
+      <c r="E82" s="220"/>
+      <c r="F82" s="220"/>
+      <c r="G82" s="220"/>
+      <c r="H82" s="220"/>
+      <c r="I82" s="220"/>
+      <c r="J82" s="220"/>
+      <c r="K82" s="220"/>
+      <c r="L82" s="220"/>
+      <c r="M82" s="220"/>
+      <c r="N82" s="220"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="220"/>
+      <c r="B86" s="220"/>
+      <c r="C86" s="220"/>
+      <c r="D86" s="220"/>
+      <c r="E86" s="220"/>
+      <c r="F86" s="220"/>
+      <c r="G86" s="220"/>
+      <c r="H86" s="220"/>
+      <c r="I86" s="220"/>
+      <c r="J86" s="220"/>
+      <c r="K86" s="220"/>
+      <c r="L86" s="220"/>
+      <c r="M86" s="220"/>
+      <c r="N86" s="220"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="221" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="223" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="223" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="224">
+        <v>56</v>
+      </c>
+      <c r="E87" s="223" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="224">
+        <v>1500</v>
+      </c>
+      <c r="G87" s="220"/>
+      <c r="H87" s="220"/>
+      <c r="I87" s="220"/>
+      <c r="J87" s="220"/>
+      <c r="K87" s="220"/>
+      <c r="L87" s="220"/>
+      <c r="M87" s="220"/>
+      <c r="N87" s="220"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" s="221">
+        <v>0</v>
+      </c>
+      <c r="B88" s="221">
+        <v>0</v>
+      </c>
+      <c r="C88" s="221">
+        <v>0</v>
+      </c>
+      <c r="D88" s="221">
+        <v>0</v>
+      </c>
+      <c r="E88" s="221">
+        <v>140</v>
+      </c>
+      <c r="F88" s="221">
+        <v>200</v>
+      </c>
+      <c r="G88" s="221">
+        <v>694</v>
+      </c>
+      <c r="H88" s="221">
+        <v>1800</v>
+      </c>
+      <c r="I88" s="221">
+        <v>0</v>
+      </c>
+      <c r="J88" s="221">
+        <v>0</v>
+      </c>
+      <c r="K88" s="239" t="s">
+        <v>128</v>
+      </c>
+      <c r="L88" s="221"/>
+      <c r="M88" s="225" t="s">
+        <v>135</v>
+      </c>
+      <c r="N88" s="221">
+        <f>B100-1+0</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" s="221">
+        <v>1</v>
+      </c>
+      <c r="B89" s="221">
+        <v>2</v>
+      </c>
+      <c r="C89" s="221">
+        <v>3</v>
+      </c>
+      <c r="D89" s="221">
+        <v>4</v>
+      </c>
+      <c r="E89" s="221">
+        <v>5</v>
+      </c>
+      <c r="F89" s="221">
+        <v>6</v>
+      </c>
+      <c r="G89" s="221">
+        <v>7</v>
+      </c>
+      <c r="H89" s="221">
+        <v>8</v>
+      </c>
+      <c r="I89" s="221">
+        <v>9</v>
+      </c>
+      <c r="J89" s="221">
+        <v>10</v>
+      </c>
+      <c r="K89" s="239"/>
+      <c r="L89" s="221"/>
+      <c r="M89" s="226" t="s">
+        <v>136</v>
+      </c>
+      <c r="N89" s="221">
+        <f>N88+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" s="221"/>
+      <c r="B90" s="221"/>
+      <c r="C90" s="221"/>
+      <c r="D90" s="221"/>
+      <c r="E90" s="221"/>
+      <c r="F90" s="221"/>
+      <c r="G90" s="221"/>
+      <c r="H90" s="221"/>
+      <c r="I90" s="221"/>
+      <c r="J90" s="221"/>
+      <c r="K90" s="221">
+        <f>SUM(A88:J88)</f>
+        <v>2834</v>
+      </c>
+      <c r="L90" s="221"/>
+      <c r="M90" s="221" t="s">
+        <v>133</v>
+      </c>
+      <c r="N90" s="221"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="221" t="s">
+        <v>130</v>
+      </c>
+      <c r="B91" s="221"/>
+      <c r="C91" s="221"/>
+      <c r="D91" s="221"/>
+      <c r="E91" s="221"/>
+      <c r="F91" s="221"/>
+      <c r="G91" s="221"/>
+      <c r="H91" s="221"/>
+      <c r="I91" s="221"/>
+      <c r="J91" s="221"/>
+      <c r="K91" s="221"/>
+      <c r="L91" s="221"/>
+      <c r="M91" s="221"/>
+      <c r="N91" s="221"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="221">
+        <f>A88+B88+C88</f>
+        <v>0</v>
+      </c>
+      <c r="B92" s="221">
+        <v>0</v>
+      </c>
+      <c r="C92" s="221">
+        <v>0</v>
+      </c>
+      <c r="D92" s="221">
+        <f>D88</f>
+        <v>0</v>
+      </c>
+      <c r="E92" s="221">
+        <f>E88+F88</f>
+        <v>340</v>
+      </c>
+      <c r="F92" s="221">
+        <f>F88</f>
+        <v>200</v>
+      </c>
+      <c r="G92" s="221">
+        <f>G88+H88</f>
+        <v>2494</v>
+      </c>
+      <c r="H92" s="221">
+        <v>0</v>
+      </c>
+      <c r="I92" s="221">
+        <f>I88+J88</f>
+        <v>0</v>
+      </c>
+      <c r="J92" s="221">
+        <v>0</v>
+      </c>
+      <c r="K92" s="221">
+        <f>SUM(A92:J92)</f>
+        <v>3034</v>
+      </c>
+      <c r="L92" s="221"/>
+      <c r="M92" s="221"/>
+      <c r="N92" s="221"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="221">
+        <v>1</v>
+      </c>
+      <c r="B93" s="221">
+        <v>2</v>
+      </c>
+      <c r="C93" s="221">
+        <v>3</v>
+      </c>
+      <c r="D93" s="221">
+        <v>4</v>
+      </c>
+      <c r="E93" s="221">
+        <v>5</v>
+      </c>
+      <c r="F93" s="221">
+        <v>6</v>
+      </c>
+      <c r="G93" s="221">
+        <v>7</v>
+      </c>
+      <c r="H93" s="221">
+        <v>8</v>
+      </c>
+      <c r="I93" s="221">
+        <v>9</v>
+      </c>
+      <c r="J93" s="221">
+        <v>10</v>
+      </c>
+      <c r="K93" s="220"/>
+      <c r="L93" s="220"/>
+      <c r="M93" s="220"/>
+      <c r="N93" s="220"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" s="220"/>
+      <c r="B94" s="220"/>
+      <c r="C94" s="220"/>
+      <c r="D94" s="220"/>
+      <c r="E94" s="220"/>
+      <c r="F94" s="220"/>
+      <c r="G94" s="220"/>
+      <c r="H94" s="220"/>
+      <c r="I94" s="220"/>
+      <c r="J94" s="220"/>
+      <c r="K94" s="220"/>
+      <c r="L94" s="220"/>
+      <c r="M94" s="220"/>
+      <c r="N94" s="220"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" s="221" t="s">
+        <v>134</v>
+      </c>
+      <c r="B95" s="220"/>
+      <c r="C95" s="220"/>
+      <c r="D95" s="220"/>
+      <c r="E95" s="220"/>
+      <c r="F95" s="220"/>
+      <c r="G95" s="220"/>
+      <c r="H95" s="220"/>
+      <c r="I95" s="220"/>
+      <c r="J95" s="220"/>
+      <c r="K95" s="221"/>
+      <c r="L95" s="221"/>
+      <c r="M95" s="221"/>
+      <c r="N95" s="221"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" s="227">
+        <v>0</v>
+      </c>
+      <c r="B96" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C96" s="221">
+        <v>1</v>
+      </c>
+      <c r="D96" s="221">
+        <v>2</v>
+      </c>
+      <c r="E96" s="221">
+        <v>3</v>
+      </c>
+      <c r="F96" s="221">
+        <v>4</v>
+      </c>
+      <c r="G96" s="221">
+        <v>5</v>
+      </c>
+      <c r="H96" s="221">
+        <v>6</v>
+      </c>
+      <c r="I96" s="221">
+        <v>7</v>
+      </c>
+      <c r="J96" s="221">
+        <v>8</v>
+      </c>
+      <c r="K96" s="221">
+        <v>9</v>
+      </c>
+      <c r="L96" s="221">
+        <v>10</v>
+      </c>
+      <c r="M96" s="221"/>
+      <c r="N96" s="221"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" s="226">
+        <v>1</v>
+      </c>
+      <c r="B97" s="221">
+        <v>1</v>
+      </c>
+      <c r="C97" s="222">
+        <v>0</v>
+      </c>
+      <c r="D97" s="222"/>
+      <c r="E97" s="222"/>
+      <c r="F97" s="222"/>
+      <c r="G97" s="222"/>
+      <c r="H97" s="222"/>
+      <c r="I97" s="222"/>
+      <c r="J97" s="222"/>
+      <c r="K97" s="222"/>
+      <c r="L97" s="222"/>
+      <c r="M97" s="243">
+        <f t="shared" ref="M97:M98" si="21">($F$49+SUM(C97:L97))/B97</f>
+        <v>1500</v>
+      </c>
+      <c r="N97" s="221"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98" s="221">
+        <v>2</v>
+      </c>
+      <c r="B98" s="221">
+        <v>2</v>
+      </c>
+      <c r="C98" s="222">
+        <f>0*B88*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D98" s="222">
+        <f>C$58*B88*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E98" s="222"/>
+      <c r="F98" s="222"/>
+      <c r="G98" s="222"/>
+      <c r="H98" s="222"/>
+      <c r="I98" s="222"/>
+      <c r="J98" s="222"/>
+      <c r="K98" s="222"/>
+      <c r="L98" s="222"/>
+      <c r="M98" s="243">
+        <f t="shared" si="21"/>
+        <v>750</v>
+      </c>
+      <c r="N98" s="221" t="str">
+        <f t="shared" ref="N98:N99" si="22">IF(M98&gt;M97,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" s="227">
+        <v>3</v>
+      </c>
+      <c r="B99" s="221">
+        <v>3</v>
+      </c>
+      <c r="C99" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D99" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E99" s="222">
+        <f>D$58*C$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="F99" s="222"/>
+      <c r="G99" s="222"/>
+      <c r="H99" s="222"/>
+      <c r="I99" s="222"/>
+      <c r="J99" s="222"/>
+      <c r="K99" s="222"/>
+      <c r="L99" s="222"/>
+      <c r="M99" s="243">
+        <f>($F$49+SUM(C99:L99))/B99</f>
+        <v>500</v>
+      </c>
+      <c r="N99" s="221" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" s="226">
+        <v>4</v>
+      </c>
+      <c r="B100" s="221">
+        <v>4</v>
+      </c>
+      <c r="C100" s="222">
+        <f>0*A$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="D100" s="222">
+        <f>C$58*B$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="E100" s="222">
+        <f>D$58*C$50*$D$49</f>
+        <v>0</v>
+      </c>
+      <c r="F100" s="222">
+        <f>E$58*D$50*$D$49</f>
+        <v>297360</v>
+      </c>
+      <c r="G100" s="222"/>
+      <c r="H100" s="222"/>
+      <c r="I100" s="222"/>
+      <c r="J100" s="222"/>
+      <c r="K100" s="222"/>
+      <c r="L100" s="222"/>
+      <c r="M100" s="243">
+        <f>($F$49+SUM(C100:L100))/B100</f>
+        <v>74715</v>
+      </c>
+      <c r="N100" s="221" t="str">
+        <f>IF(M100&gt;M99,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="221"/>
+      <c r="B101" s="221"/>
+      <c r="C101" s="222"/>
+      <c r="D101" s="222"/>
+      <c r="E101" s="222"/>
+      <c r="F101" s="222"/>
+      <c r="G101" s="222"/>
+      <c r="H101" s="222"/>
+      <c r="I101" s="222"/>
+      <c r="J101" s="222"/>
+      <c r="K101" s="222"/>
+      <c r="L101" s="222"/>
+      <c r="M101" s="222"/>
+      <c r="N101" s="221"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B102" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C102" s="221">
+        <v>1</v>
+      </c>
+      <c r="D102" s="221">
+        <v>2</v>
+      </c>
+      <c r="E102" s="221">
+        <v>3</v>
+      </c>
+      <c r="F102" s="221">
+        <v>4</v>
+      </c>
+      <c r="G102" s="221">
+        <v>5</v>
+      </c>
+      <c r="H102" s="221">
+        <v>6</v>
+      </c>
+      <c r="I102" s="221">
+        <v>7</v>
+      </c>
+      <c r="J102" s="221">
+        <v>8</v>
+      </c>
+      <c r="K102" s="221">
+        <v>9</v>
+      </c>
+      <c r="L102" s="221">
+        <v>10</v>
+      </c>
+      <c r="M102" s="221"/>
+      <c r="N102" s="221"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" s="227">
+        <v>4</v>
+      </c>
+      <c r="B103" s="221">
+        <v>1</v>
+      </c>
+      <c r="C103" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D103" s="222"/>
+      <c r="E103" s="222"/>
+      <c r="F103" s="222"/>
+      <c r="G103" s="222"/>
+      <c r="H103" s="222"/>
+      <c r="I103" s="222"/>
+      <c r="J103" s="222"/>
+      <c r="K103" s="222"/>
+      <c r="L103" s="222"/>
+      <c r="M103" s="243">
+        <f t="shared" ref="M103:M104" si="23">($F$49+SUM(C103:L103))/B103</f>
+        <v>1500</v>
+      </c>
+      <c r="N103" s="221"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="226">
+        <v>5</v>
+      </c>
+      <c r="B104" s="221">
+        <v>2</v>
+      </c>
+      <c r="C104" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D104" s="222">
+        <f>E$50*$D$49*C$64</f>
+        <v>100800</v>
+      </c>
+      <c r="E104" s="222"/>
+      <c r="F104" s="222"/>
+      <c r="G104" s="222"/>
+      <c r="H104" s="222"/>
+      <c r="I104" s="222"/>
+      <c r="J104" s="222"/>
+      <c r="K104" s="222"/>
+      <c r="L104" s="222"/>
+      <c r="M104" s="243">
+        <f>($F$49+SUM(C104:L104))/B104</f>
+        <v>51150</v>
+      </c>
+      <c r="N104" s="221" t="str">
+        <f t="shared" ref="N104" si="24">IF(M104&gt;M103,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" s="221"/>
+      <c r="B105" s="221"/>
+      <c r="C105" s="222"/>
+      <c r="D105" s="222"/>
+      <c r="E105" s="222"/>
+      <c r="F105" s="222"/>
+      <c r="G105" s="222"/>
+      <c r="H105" s="222"/>
+      <c r="I105" s="222"/>
+      <c r="J105" s="222"/>
+      <c r="K105" s="222"/>
+      <c r="L105" s="222"/>
+      <c r="M105" s="222"/>
+      <c r="N105" s="221"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B106" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C106" s="221">
+        <v>1</v>
+      </c>
+      <c r="D106" s="221">
+        <v>2</v>
+      </c>
+      <c r="E106" s="221">
+        <v>3</v>
+      </c>
+      <c r="F106" s="221">
+        <v>4</v>
+      </c>
+      <c r="G106" s="221">
+        <v>5</v>
+      </c>
+      <c r="H106" s="221">
+        <v>6</v>
+      </c>
+      <c r="I106" s="221">
+        <v>7</v>
+      </c>
+      <c r="J106" s="221">
+        <v>8</v>
+      </c>
+      <c r="K106" s="221">
+        <v>9</v>
+      </c>
+      <c r="L106" s="221">
+        <v>10</v>
+      </c>
+      <c r="M106" s="221"/>
+      <c r="N106" s="221"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A107" s="221">
+        <v>5</v>
+      </c>
+      <c r="B107" s="221">
+        <v>1</v>
+      </c>
+      <c r="C107" s="222">
+        <v>0</v>
+      </c>
+      <c r="D107" s="222"/>
+      <c r="E107" s="222"/>
+      <c r="F107" s="222"/>
+      <c r="G107" s="222"/>
+      <c r="H107" s="222"/>
+      <c r="I107" s="222"/>
+      <c r="J107" s="222"/>
+      <c r="K107" s="222"/>
+      <c r="L107" s="222"/>
+      <c r="M107" s="243">
+        <f t="shared" ref="M107:M109" si="25">($F$49+SUM(C107:L107))/B107</f>
+        <v>1500</v>
+      </c>
+      <c r="N107" s="221"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A108" s="227">
+        <v>6</v>
+      </c>
+      <c r="B108" s="221">
+        <v>2</v>
+      </c>
+      <c r="C108" s="222">
+        <v>0</v>
+      </c>
+      <c r="D108" s="222">
+        <f>F$50*$D$49*C$68</f>
+        <v>0</v>
+      </c>
+      <c r="E108" s="222"/>
+      <c r="F108" s="222"/>
+      <c r="G108" s="222"/>
+      <c r="H108" s="222"/>
+      <c r="I108" s="222"/>
+      <c r="J108" s="222"/>
+      <c r="K108" s="222"/>
+      <c r="L108" s="222"/>
+      <c r="M108" s="243">
+        <f t="shared" si="25"/>
+        <v>750</v>
+      </c>
+      <c r="N108" s="221" t="str">
+        <f>IF(M108&gt;M107,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A109" s="226">
+        <v>7</v>
+      </c>
+      <c r="B109" s="221">
+        <v>3</v>
+      </c>
+      <c r="C109" s="222">
+        <v>0</v>
+      </c>
+      <c r="D109" s="222">
+        <f>F$50*$D$49*C$68</f>
+        <v>0</v>
+      </c>
+      <c r="E109" s="222">
+        <f>G$50*$D$49*D$68</f>
+        <v>134400</v>
+      </c>
+      <c r="F109" s="222"/>
+      <c r="G109" s="222"/>
+      <c r="H109" s="222"/>
+      <c r="I109" s="222"/>
+      <c r="J109" s="222"/>
+      <c r="K109" s="222"/>
+      <c r="L109" s="222"/>
+      <c r="M109" s="243">
+        <f t="shared" si="25"/>
+        <v>45300</v>
+      </c>
+      <c r="N109" s="221" t="str">
+        <f>IF(M109&gt;M108,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" s="221"/>
+      <c r="B110" s="221"/>
+      <c r="C110" s="222"/>
+      <c r="D110" s="222"/>
+      <c r="E110" s="222"/>
+      <c r="F110" s="222"/>
+      <c r="G110" s="222"/>
+      <c r="H110" s="222"/>
+      <c r="I110" s="222"/>
+      <c r="J110" s="222"/>
+      <c r="K110" s="222"/>
+      <c r="L110" s="222"/>
+      <c r="M110" s="222"/>
+      <c r="N110" s="221"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B111" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C111" s="221">
+        <v>1</v>
+      </c>
+      <c r="D111" s="221">
+        <v>2</v>
+      </c>
+      <c r="E111" s="221">
+        <v>3</v>
+      </c>
+      <c r="F111" s="221">
+        <v>4</v>
+      </c>
+      <c r="G111" s="221">
+        <v>5</v>
+      </c>
+      <c r="H111" s="221">
+        <v>6</v>
+      </c>
+      <c r="I111" s="221">
+        <v>7</v>
+      </c>
+      <c r="J111" s="221">
+        <v>8</v>
+      </c>
+      <c r="K111" s="221">
+        <v>9</v>
+      </c>
+      <c r="L111" s="221">
+        <v>10</v>
+      </c>
+      <c r="M111" s="221"/>
+      <c r="N111" s="221"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A112" s="221">
+        <v>7</v>
+      </c>
+      <c r="B112" s="221">
+        <v>1</v>
+      </c>
+      <c r="C112" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D112" s="222"/>
+      <c r="E112" s="222"/>
+      <c r="F112" s="222"/>
+      <c r="G112" s="222"/>
+      <c r="H112" s="222"/>
+      <c r="I112" s="222"/>
+      <c r="J112" s="222"/>
+      <c r="K112" s="222"/>
+      <c r="L112" s="222"/>
+      <c r="M112" s="243">
+        <f t="shared" ref="M112:M114" si="26">($F$49+SUM(C112:L112))/B112</f>
+        <v>1500</v>
+      </c>
+      <c r="N112" s="221"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A113" s="227">
+        <v>8</v>
+      </c>
+      <c r="B113" s="221">
+        <v>2</v>
+      </c>
+      <c r="C113" s="222">
+        <v>0</v>
+      </c>
+      <c r="D113" s="222">
+        <f>H$50*$D$49*C$73</f>
+        <v>0</v>
+      </c>
+      <c r="E113" s="222"/>
+      <c r="F113" s="222"/>
+      <c r="G113" s="222"/>
+      <c r="H113" s="222"/>
+      <c r="I113" s="222"/>
+      <c r="J113" s="222"/>
+      <c r="K113" s="222"/>
+      <c r="L113" s="222"/>
+      <c r="M113" s="243">
+        <f t="shared" si="26"/>
+        <v>750</v>
+      </c>
+      <c r="N113" s="221" t="str">
+        <f>IF(M113&gt;M112,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A114" s="226">
+        <v>9</v>
+      </c>
+      <c r="B114" s="221">
+        <v>3</v>
+      </c>
+      <c r="C114" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D114" s="222">
+        <f>H$50*$D$49*C$73</f>
+        <v>0</v>
+      </c>
+      <c r="E114" s="222">
+        <f>I$50*$D$49*D$73</f>
+        <v>67200</v>
+      </c>
+      <c r="F114" s="222"/>
+      <c r="G114" s="222"/>
+      <c r="H114" s="222"/>
+      <c r="I114" s="222"/>
+      <c r="J114" s="222"/>
+      <c r="K114" s="222"/>
+      <c r="L114" s="222"/>
+      <c r="M114" s="243">
+        <f t="shared" si="26"/>
+        <v>22900</v>
+      </c>
+      <c r="N114" s="221" t="str">
+        <f>IF(M114&gt;M113,"YA","")</f>
+        <v>YA</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A115" s="221"/>
+      <c r="B115" s="221"/>
+      <c r="C115" s="222"/>
+      <c r="D115" s="222"/>
+      <c r="E115" s="222"/>
+      <c r="F115" s="222"/>
+      <c r="G115" s="222"/>
+      <c r="H115" s="222"/>
+      <c r="I115" s="222"/>
+      <c r="J115" s="222"/>
+      <c r="K115" s="222"/>
+      <c r="L115" s="222"/>
+      <c r="M115" s="222"/>
+      <c r="N115" s="221"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A116" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="B116" s="221" t="s">
+        <v>129</v>
+      </c>
+      <c r="C116" s="221">
+        <v>1</v>
+      </c>
+      <c r="D116" s="221">
+        <v>2</v>
+      </c>
+      <c r="E116" s="221">
+        <v>3</v>
+      </c>
+      <c r="F116" s="221">
+        <v>4</v>
+      </c>
+      <c r="G116" s="221">
+        <v>5</v>
+      </c>
+      <c r="H116" s="221">
+        <v>6</v>
+      </c>
+      <c r="I116" s="221">
+        <v>7</v>
+      </c>
+      <c r="J116" s="221">
+        <v>8</v>
+      </c>
+      <c r="K116" s="221">
+        <v>9</v>
+      </c>
+      <c r="L116" s="221">
+        <v>10</v>
+      </c>
+      <c r="M116" s="221"/>
+      <c r="N116" s="221"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A117" s="221">
+        <v>9</v>
+      </c>
+      <c r="B117" s="221">
+        <v>1</v>
+      </c>
+      <c r="C117" s="222">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D117" s="222"/>
+      <c r="E117" s="222"/>
+      <c r="F117" s="222"/>
+      <c r="G117" s="222"/>
+      <c r="H117" s="222"/>
+      <c r="I117" s="222"/>
+      <c r="J117" s="222"/>
+      <c r="K117" s="222"/>
+      <c r="L117" s="222"/>
+      <c r="M117" s="222">
+        <f t="shared" ref="M117:M118" si="27">($F$49+SUM(C117:L117))/B117</f>
+        <v>1500</v>
+      </c>
+      <c r="N117" s="221"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A118" s="227">
+        <v>10</v>
+      </c>
+      <c r="B118" s="221">
+        <v>2</v>
+      </c>
+      <c r="C118" s="222">
+        <v>0</v>
+      </c>
+      <c r="D118" s="222">
+        <f>J$50*$D$49*C$78</f>
+        <v>0</v>
+      </c>
+      <c r="E118" s="222"/>
+      <c r="F118" s="222"/>
+      <c r="G118" s="222"/>
+      <c r="H118" s="222"/>
+      <c r="I118" s="222"/>
+      <c r="J118" s="222"/>
+      <c r="K118" s="222"/>
+      <c r="L118" s="222"/>
+      <c r="M118" s="222">
+        <f t="shared" si="27"/>
+        <v>750</v>
+      </c>
+      <c r="N118" s="221" t="str">
+        <f>IF(M118&gt;M117,"YA","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A119" s="221"/>
+      <c r="B119" s="221"/>
+      <c r="C119" s="222"/>
+      <c r="D119" s="222"/>
+      <c r="E119" s="222"/>
+      <c r="F119" s="222"/>
+      <c r="G119" s="222"/>
+      <c r="H119" s="222"/>
+      <c r="I119" s="222"/>
+      <c r="J119" s="222"/>
+      <c r="K119" s="222"/>
+      <c r="L119" s="222"/>
+      <c r="M119" s="222"/>
+      <c r="N119" s="221"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A120" s="220"/>
+      <c r="B120" s="220"/>
+      <c r="C120" s="220"/>
+      <c r="D120" s="220"/>
+      <c r="E120" s="220"/>
+      <c r="F120" s="220"/>
+      <c r="G120" s="220"/>
+      <c r="H120" s="220"/>
+      <c r="I120" s="220"/>
+      <c r="J120" s="220"/>
+      <c r="K120" s="220"/>
+      <c r="L120" s="220"/>
+      <c r="M120" s="220"/>
+      <c r="N120" s="220"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="K88:K89"/>
+    <mergeCell ref="W50:W51"/>
+    <mergeCell ref="K50:K51"/>
     <mergeCell ref="P7:R7"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="C7:E7"/>
@@ -16506,6 +18676,8 @@
     <mergeCell ref="H27:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>